<commit_message>
Added a LINQ Where Benchmark
</commit_message>
<xml_diff>
--- a/ArrayVsDictionaryBenchmark.xlsx
+++ b/ArrayVsDictionaryBenchmark.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27375" windowHeight="10500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27375" windowHeight="10500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="VaueType Array-Dictionary" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="String Concatention" sheetId="5" r:id="rId4"/>
     <sheet name="TableValuedParameters" sheetId="4" r:id="rId5"/>
     <sheet name="SlugProducer" sheetId="6" r:id="rId6"/>
+    <sheet name="LinqWhere" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Sorted Array</t>
   </si>
@@ -166,12 +167,51 @@
   <si>
     <t>ABCDEFGHIJKLMNOPQRSTUVWXYZ0123456789 .-" + "–"</t>
   </si>
+  <si>
+    <t>GetUsingMultipleToUpper</t>
+  </si>
+  <si>
+    <t>GetUsingMultipleEqualityComparer</t>
+  </si>
+  <si>
+    <t>GetUsingConcatAndMultipleToUpper</t>
+  </si>
+  <si>
+    <t>GetUsingQueryExpLetAndOneToUpper</t>
+  </si>
+  <si>
+    <t>GetUsingLocalvariableAssignmentForToUpper</t>
+  </si>
+  <si>
+    <t>GetWithoutLINQ</t>
+  </si>
+  <si>
+    <t>GetWithoutLINQNoToUpper</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Gen 0</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>Allocated Bytes</t>
+  </si>
+  <si>
+    <t>Mean (ns)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,13 +268,6 @@
       <color theme="0"/>
       <name val="Segoe UI Light"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -342,6 +375,33 @@
       <name val="Segoe UI Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -412,7 +472,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,44 +488,194 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="4" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="4" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="22" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="22" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="23" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="4" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -11495,6 +11705,21 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Benchmark" dataDxfId="7"/>
+    <tableColumn id="2" name="Mean (ns)" dataDxfId="6"/>
+    <tableColumn id="3" name="Ratio" dataDxfId="5"/>
+    <tableColumn id="4" name="Rank" dataDxfId="4"/>
+    <tableColumn id="5" name="Gen 0" dataDxfId="3"/>
+    <tableColumn id="6" name="Allocated Bytes" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11800,269 +12025,269 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="25.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="25">
+      <c r="B2" s="23">
         <v>5</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="23">
         <v>10</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="23">
         <v>15</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="23">
         <v>20</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="23">
         <v>25</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="23">
         <v>30</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="23">
         <v>35</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="23">
         <v>40</v>
       </c>
-      <c r="J2" s="25">
+      <c r="J2" s="23">
         <v>45</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="23">
         <v>50</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="23">
         <v>55</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="23">
         <v>60</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="23">
         <v>65</v>
       </c>
-      <c r="O2" s="25">
+      <c r="O2" s="23">
         <v>70</v>
       </c>
-      <c r="P2" s="25">
+      <c r="P2" s="23">
         <v>75</v>
       </c>
-      <c r="Q2" s="25">
+      <c r="Q2" s="23">
         <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="25">
         <v>15.73</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="25">
         <v>54.49</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="25">
         <v>119.56</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="25">
         <v>230.24</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="25">
         <v>328.7</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="25">
         <v>498.11</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="26">
         <v>706.84</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="26">
         <v>935.54</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="27">
         <v>1229.3800000000001</v>
       </c>
-      <c r="K3" s="30">
+      <c r="K3" s="28">
         <v>1495.37</v>
       </c>
-      <c r="L3" s="29">
+      <c r="L3" s="27">
         <v>1884.6</v>
       </c>
-      <c r="M3" s="29">
+      <c r="M3" s="27">
         <v>2253.4</v>
       </c>
-      <c r="N3" s="29">
+      <c r="N3" s="27">
         <v>2653.5</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="27">
         <v>3054.3</v>
       </c>
-      <c r="P3" s="29">
+      <c r="P3" s="27">
         <v>3488.1</v>
       </c>
-      <c r="Q3" s="29">
+      <c r="Q3" s="27">
         <v>4024.3</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="26">
         <v>69</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="29">
         <v>178.29</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="29">
         <v>299.27</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="29">
         <v>421.2</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="29">
         <v>568.62</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="29">
         <v>682.98</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="29">
         <v>828.24</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="28">
         <v>979.91</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="28">
         <v>1132.77</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4" s="27">
         <v>1271.56</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="27">
         <v>1463</v>
       </c>
-      <c r="M4" s="29">
+      <c r="M4" s="27">
         <v>1613.1</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="27">
         <v>1737.2</v>
       </c>
-      <c r="O4" s="29">
+      <c r="O4" s="27">
         <v>1964.6</v>
       </c>
-      <c r="P4" s="29">
+      <c r="P4" s="27">
         <v>2152.1</v>
       </c>
-      <c r="Q4" s="29">
+      <c r="Q4" s="27">
         <v>2303.1999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="26">
         <v>42.58</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="26">
         <v>101.48</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="26">
         <v>157.25</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="30">
         <v>206.18</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="26">
         <v>249.16</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="26">
         <v>313.43</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="26">
         <v>384.29</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="26">
         <v>416.34</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="26">
         <v>521.36</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="26">
         <v>703.1</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="26">
         <v>613.4</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="26">
         <v>686.2</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="26">
         <v>707</v>
       </c>
-      <c r="O5" s="28">
+      <c r="O5" s="26">
         <v>759.4</v>
       </c>
-      <c r="P5" s="28">
+      <c r="P5" s="26">
         <v>860.4</v>
       </c>
-      <c r="Q5" s="28">
+      <c r="Q5" s="26">
         <v>962.1</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="29">
         <v>77.91</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="26">
         <v>166.23</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="26">
         <v>267.25</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="26">
         <v>361.71</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="26">
         <v>491.72</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="26">
         <v>568.28</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="25">
         <v>690.62</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="25">
         <v>773.99</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="25">
         <v>862.26</v>
       </c>
-      <c r="K6" s="33">
+      <c r="K6" s="31">
         <v>1077.33</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="27">
         <v>1120.7</v>
       </c>
-      <c r="M6" s="29">
+      <c r="M6" s="27">
         <v>1155.9000000000001</v>
       </c>
-      <c r="N6" s="29">
+      <c r="N6" s="27">
         <v>1306.3</v>
       </c>
-      <c r="O6" s="29">
+      <c r="O6" s="27">
         <v>1461.2</v>
       </c>
-      <c r="P6" s="29">
+      <c r="P6" s="27">
         <v>1592.1</v>
       </c>
-      <c r="Q6" s="29">
+      <c r="Q6" s="27">
         <v>1590.8</v>
       </c>
     </row>
@@ -12473,178 +12698,178 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="12"/>
-    <col min="10" max="10" width="9.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="32" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="34"/>
+    <col min="10" max="10" width="9.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="32">
         <v>10</v>
       </c>
-      <c r="C1" s="10">
+      <c r="C1" s="32">
         <v>100</v>
       </c>
-      <c r="D1" s="10">
+      <c r="D1" s="32">
         <v>200</v>
       </c>
-      <c r="E1" s="10">
+      <c r="E1" s="32">
         <v>300</v>
       </c>
-      <c r="F1" s="11">
+      <c r="F1" s="33">
         <v>500</v>
       </c>
-      <c r="G1" s="11">
+      <c r="G1" s="33">
         <v>1000</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="36">
         <v>1.446</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="36">
         <v>1.47</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="36">
         <v>1.514</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="36">
         <v>1.4410000000000001</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="36">
         <v>1.647</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="36">
         <v>1.5389999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="36">
         <v>1.3680000000000001</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="36">
         <v>1.5089999999999999</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="36">
         <v>1.6419999999999999</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="36">
         <v>1.62</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="36">
         <v>1.6439999999999999</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="36">
         <v>1.556</v>
       </c>
-      <c r="H3" s="14"/>
+      <c r="H3" s="36"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="36">
         <v>14.057</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="36">
         <v>12.813000000000001</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="36">
         <v>13.53</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="36">
         <v>12.962999999999999</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="36">
         <v>13.013</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="36">
         <v>12.465</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="36">
         <v>13.779</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="36">
         <v>12.997</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="36">
         <v>14.000999999999999</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="36">
         <v>12.867000000000001</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="36">
         <v>12.904</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="36">
         <v>12.762</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="36">
         <v>1.7669999999999999</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="36">
         <v>2.125</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="36">
         <v>2.3359999999999999</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="36">
         <v>2.0299999999999998</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="36">
         <v>1.9510000000000001</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="36">
         <v>2.052</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="36">
         <v>12.372</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="36">
         <v>13.018000000000001</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="36">
         <v>14.196999999999999</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="36">
         <v>12.509</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="36">
         <v>12.648</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="36">
         <v>12.743</v>
       </c>
     </row>
@@ -12664,260 +12889,260 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="19.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="16">
+      <c r="B1" s="14">
         <v>2</v>
       </c>
-      <c r="C1" s="16">
+      <c r="C1" s="14">
         <v>3</v>
       </c>
-      <c r="D1" s="16">
+      <c r="D1" s="14">
         <v>4</v>
       </c>
-      <c r="E1" s="16">
+      <c r="E1" s="14">
         <v>5</v>
       </c>
-      <c r="F1" s="16">
+      <c r="F1" s="14">
         <v>6</v>
       </c>
-      <c r="G1" s="16">
+      <c r="G1" s="14">
         <v>7</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="14">
         <v>8</v>
       </c>
-      <c r="I1" s="16">
+      <c r="I1" s="14">
         <v>9</v>
       </c>
-      <c r="J1" s="16">
+      <c r="J1" s="14">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="16">
         <v>35.18</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="16">
         <v>48.49</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="16">
         <v>63.77</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="16">
         <v>100.7</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="16">
         <v>116.58</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="16">
         <v>147.13999999999999</v>
       </c>
-      <c r="H2" s="18">
+      <c r="H2" s="16">
         <v>188</v>
       </c>
-      <c r="I2" s="18">
+      <c r="I2" s="16">
         <v>201.92</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="16">
         <v>202.92</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <v>36.770000000000003</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="16">
         <v>79.45</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="16">
         <v>130.53</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="16">
         <v>190.99</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="16">
         <v>256.54000000000002</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="16">
         <v>358.8</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="16">
         <v>488.48</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="16">
         <v>559.79999999999995</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="16">
         <v>651.79</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>37.15</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>48.36</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <v>62.73</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="16">
         <v>81.739999999999995</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="16">
         <v>100.52</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="16">
         <v>121.92</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="16">
         <v>137</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="16">
         <v>171.35</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="16">
         <v>177.58</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>36.89</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>80.849999999999994</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>129.88999999999999</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="16">
         <v>212.4</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="16">
         <v>324.85000000000002</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="16">
         <v>400.4</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="16">
         <v>448.09</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="16">
         <v>657.48</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="16">
         <v>700.75</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>133.80000000000001</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>191.67</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>212.86</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <v>285.92</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="16">
         <v>326.55</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="16">
         <v>350.79</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="16">
         <v>366.17</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="16">
         <v>504.34</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="16">
         <v>464.81</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>132.9</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>193.09</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>217.53</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <v>289.44</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="16">
         <v>332.43</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="16">
         <v>350.39</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="16">
         <v>368.79</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <v>523.46</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="16">
         <v>475.01</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <v>51.35</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <v>67.06</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>88.24</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <v>100.33</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="16">
         <v>128.13</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="16">
         <v>149.41999999999999</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="16">
         <v>165.35</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="16">
         <v>194.97</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="16">
         <v>197.98</v>
       </c>
     </row>
@@ -13013,357 +13238,357 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="12">
         <v>14.304</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="12">
         <v>14.541</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="12">
         <v>15.433</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="12">
         <v>15.71</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="12">
         <v>16.486999999999998</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="12">
         <v>17.047999999999998</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="12">
         <v>19.948</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="12">
         <v>26.03</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="12">
         <v>30.724</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="12">
         <v>36.429000000000002</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="12">
         <v>41.828000000000003</v>
       </c>
-      <c r="M2" s="14">
+      <c r="M2" s="12">
         <v>46.32</v>
       </c>
-      <c r="N2" s="14">
+      <c r="N2" s="12">
         <v>50.433999999999997</v>
       </c>
-      <c r="O2" s="14">
+      <c r="O2" s="12">
         <v>56.555999999999997</v>
       </c>
-      <c r="P2" s="14">
+      <c r="P2" s="12">
         <v>59.514000000000003</v>
       </c>
-      <c r="Q2" s="14">
+      <c r="Q2" s="12">
         <v>64.555000000000007</v>
       </c>
-      <c r="R2" s="14">
+      <c r="R2" s="12">
         <v>107.473</v>
       </c>
-      <c r="S2" s="14">
+      <c r="S2" s="12">
         <v>153.93</v>
       </c>
-      <c r="T2" s="14">
+      <c r="T2" s="12">
         <v>197.583</v>
       </c>
-      <c r="U2" s="14">
+      <c r="U2" s="12">
         <v>249.49700000000001</v>
       </c>
-      <c r="V2" s="14">
+      <c r="V2" s="12">
         <v>679.07600000000002</v>
       </c>
-      <c r="W2" s="14">
+      <c r="W2" s="12">
         <v>47361.822999999997</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="12">
         <v>12.749000000000001</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="12">
         <v>12.847</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="12">
         <v>13.179</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="12">
         <v>13.566000000000001</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="12">
         <v>14</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="12">
         <v>14.515000000000001</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="12">
         <v>17.687000000000001</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="12">
         <v>23.503</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="12">
         <v>28.215</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="12">
         <v>33.960999999999999</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="12">
         <v>38.426000000000002</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="12">
         <v>43.427</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="12">
         <v>48.953000000000003</v>
       </c>
-      <c r="O3" s="14">
+      <c r="O3" s="12">
         <v>53.048000000000002</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="12">
         <v>59.817999999999998</v>
       </c>
-      <c r="Q3" s="14">
+      <c r="Q3" s="12">
         <v>61.57</v>
       </c>
-      <c r="R3" s="14">
+      <c r="R3" s="12">
         <v>107.59699999999999</v>
       </c>
-      <c r="S3" s="14">
+      <c r="S3" s="12">
         <v>148.767</v>
       </c>
-      <c r="T3" s="14">
+      <c r="T3" s="12">
         <v>193.00299999999999</v>
       </c>
-      <c r="U3" s="14">
+      <c r="U3" s="12">
         <v>241.80099999999999</v>
       </c>
-      <c r="V3" s="14">
+      <c r="V3" s="12">
         <v>630.86</v>
       </c>
-      <c r="W3" s="14">
+      <c r="W3" s="12">
         <v>46784.144999999997</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="12">
         <v>10.973000000000001</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="12">
         <v>11.3</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>11.881</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>12.253</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="12">
         <v>13.228999999999999</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="12">
         <v>13.244999999999999</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="12">
         <v>16.024000000000001</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="12">
         <v>22.306000000000001</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="12">
         <v>26.614999999999998</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="12">
         <v>33.057000000000002</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="12">
         <v>36.984999999999999</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="12">
         <v>44.848999999999997</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="12">
         <v>46.399000000000001</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="12">
         <v>50.713000000000001</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="12">
         <v>57.05</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="Q4" s="12">
         <v>60.966999999999999</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="12">
         <v>107.334</v>
       </c>
-      <c r="S4" s="14">
+      <c r="S4" s="12">
         <v>146.124</v>
       </c>
-      <c r="T4" s="14">
+      <c r="T4" s="12">
         <v>192.298</v>
       </c>
-      <c r="U4" s="14">
+      <c r="U4" s="12">
         <v>247.01</v>
       </c>
-      <c r="V4" s="14">
+      <c r="V4" s="12">
         <v>630.53</v>
       </c>
-      <c r="W4" s="14">
+      <c r="W4" s="12">
         <v>47061.86</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="12">
         <v>6.2030000000000003</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="12">
         <v>6.4989999999999997</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>7.4809999999999999</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>8.8160000000000007</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>9.3369999999999997</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="12">
         <v>10.241</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="12">
         <v>15.241</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="12">
         <v>24.901</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="12">
         <v>34.351999999999997</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="12">
         <v>43.749000000000002</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="12">
         <v>54.134999999999998</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="12">
         <v>62.235999999999997</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="12">
         <v>71.62</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="12">
         <v>81.510000000000005</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="12">
         <v>99.635000000000005</v>
       </c>
-      <c r="Q5" s="14">
+      <c r="Q5" s="12">
         <v>102.164</v>
       </c>
-      <c r="R5" s="14">
+      <c r="R5" s="12">
         <v>200.52799999999999</v>
       </c>
-      <c r="S5" s="14">
+      <c r="S5" s="12">
         <v>298.84100000000001</v>
       </c>
-      <c r="T5" s="14">
+      <c r="T5" s="12">
         <v>391.67099999999999</v>
       </c>
-      <c r="U5" s="14">
+      <c r="U5" s="12">
         <v>492.51100000000002</v>
       </c>
-      <c r="V5" s="14">
+      <c r="V5" s="12">
         <v>1148.0239999999999</v>
       </c>
-      <c r="W5" s="14">
+      <c r="W5" s="12">
         <v>106204.17</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>4.6230000000000002</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="12">
         <v>5.8410000000000002</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>8.3849999999999998</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="12">
         <v>10.641</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="12">
         <v>12.015000000000001</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <v>13.756</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="12">
         <v>22.65</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="12">
         <v>34.552</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="12">
         <v>49.610999999999997</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="12">
         <v>65.718000000000004</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="12">
         <v>81.837999999999994</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="12">
         <v>93.968000000000004</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="12">
         <v>108.58799999999999</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="12">
         <v>122.69499999999999</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="12">
         <v>142.553</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="Q6" s="12">
         <v>154.23500000000001</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6" s="12">
         <v>299.49599999999998</v>
       </c>
-      <c r="S6" s="14">
+      <c r="S6" s="12">
         <v>439.22</v>
       </c>
-      <c r="T6" s="14">
+      <c r="T6" s="12">
         <v>598.00800000000004</v>
       </c>
-      <c r="U6" s="14">
+      <c r="U6" s="12">
         <v>733.58799999999997</v>
       </c>
-      <c r="V6" s="14">
+      <c r="V6" s="12">
         <v>1680.845</v>
       </c>
-      <c r="W6" s="14">
+      <c r="W6" s="12">
         <v>155452.527</v>
       </c>
     </row>
@@ -13383,172 +13608,172 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="19"/>
-    <col min="10" max="10" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="96.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="20.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="17"/>
+    <col min="10" max="10" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="96.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="20">
         <v>1392.5</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="20">
         <v>2096.6</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="20">
         <v>2019.6</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="20">
         <v>1071.5999999999999</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="20">
         <v>1180.3</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="20">
         <v>1161.4000000000001</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="20">
         <v>960.3</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="20">
         <v>2160.3000000000002</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="20">
         <v>3576.3</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="20">
         <v>3389.1</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="20">
         <v>2008</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="20">
         <v>1738.4</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="20">
         <v>1937.7</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="20">
         <v>1663.2</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="20">
         <v>1042.5</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="20">
         <v>1899.6</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="20">
         <v>1836.4</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="20">
         <v>885</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="20">
         <v>840.9</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="20">
         <v>989.2</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="20">
         <v>777.4</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="21" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="21" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="K11" s="21" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J12" s="20" t="s">
+      <c r="J12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="21" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="21" t="s">
         <v>44</v>
       </c>
     </row>
@@ -13558,4 +13783,190 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1142.5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="4">
+        <v>890.7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8.9599999999999999E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1884.4</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.65</v>
+      </c>
+      <c r="D4" s="4">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.18310000000000001</v>
+      </c>
+      <c r="F4" s="4">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="4">
+        <v>828.8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>9.35E-2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="4">
+        <v>689.6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5.5300000000000002E-2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="4">
+        <v>564.6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="4">
+        <v>186.5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a new StringMutate vs Concat benchmark and added Gen0 and Allocations columns to Excel spreadsheet
</commit_message>
<xml_diff>
--- a/ArrayVsDictionaryBenchmark.xlsx
+++ b/ArrayVsDictionaryBenchmark.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c102116\Source\Repos\VariousBenchmarks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivk\source\repos\matlus\VariousBenchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FF1ED4-868E-4C6E-9250-A7A01052BA8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27375" windowHeight="10500" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VaueType Array-Dictionary" sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>Sorted Array</t>
   </si>
@@ -206,11 +207,32 @@
   <si>
     <t>Mean (ns)</t>
   </si>
+  <si>
+    <t>Gen0</t>
+  </si>
+  <si>
+    <t>Alloc</t>
+  </si>
+  <si>
+    <t>1136 B</t>
+  </si>
+  <si>
+    <t>5672 B</t>
+  </si>
+  <si>
+    <t>1032 B</t>
+  </si>
+  <si>
+    <t>3072 B</t>
+  </si>
+  <si>
+    <t>1048 B</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,7 +494,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -524,6 +546,9 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="4" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -3978,31 +4003,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>35.18</c:v>
+                  <c:v>30.31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.49</c:v>
+                  <c:v>43.51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.77</c:v>
+                  <c:v>63.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.7</c:v>
+                  <c:v>90.85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>116.58</c:v>
+                  <c:v>103.37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>147.13999999999999</c:v>
+                  <c:v>123.32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>188</c:v>
+                  <c:v>135.19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>201.92</c:v>
+                  <c:v>148.81</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>202.92</c:v>
+                  <c:v>181.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4083,31 +4108,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>36.770000000000003</c:v>
+                  <c:v>31.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79.45</c:v>
+                  <c:v>68.36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130.53</c:v>
+                  <c:v>124.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>190.99</c:v>
+                  <c:v>165.77</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256.54000000000002</c:v>
+                  <c:v>238.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>358.8</c:v>
+                  <c:v>331.89</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>488.48</c:v>
+                  <c:v>384.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>559.79999999999995</c:v>
+                  <c:v>464.51</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>651.79</c:v>
+                  <c:v>550.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4188,31 +4213,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>37.15</c:v>
+                  <c:v>30.14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.36</c:v>
+                  <c:v>42.61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.73</c:v>
+                  <c:v>60.26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81.739999999999995</c:v>
+                  <c:v>74.87</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.52</c:v>
+                  <c:v>92.47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121.92</c:v>
+                  <c:v>105.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>137</c:v>
+                  <c:v>113.45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>171.35</c:v>
+                  <c:v>125.57</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>177.58</c:v>
+                  <c:v>154.71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4293,31 +4318,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>36.89</c:v>
+                  <c:v>31.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.849999999999994</c:v>
+                  <c:v>68.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>129.88999999999999</c:v>
+                  <c:v>117.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>212.4</c:v>
+                  <c:v>171.78</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>324.85000000000002</c:v>
+                  <c:v>228.46</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>400.4</c:v>
+                  <c:v>295.26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>448.09</c:v>
+                  <c:v>373.92</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>657.48</c:v>
+                  <c:v>457.44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>700.75</c:v>
+                  <c:v>564.54999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4398,31 +4423,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>133.80000000000001</c:v>
+                  <c:v>116.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>191.67</c:v>
+                  <c:v>167.63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>212.86</c:v>
+                  <c:v>203.84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>285.92</c:v>
+                  <c:v>255.88</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>326.55</c:v>
+                  <c:v>273.02</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>350.79</c:v>
+                  <c:v>284.45999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>366.17</c:v>
+                  <c:v>303.91000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>504.34</c:v>
+                  <c:v>386.91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>464.81</c:v>
+                  <c:v>405.28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4503,31 +4528,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>132.9</c:v>
+                  <c:v>116.51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>193.09</c:v>
+                  <c:v>166.51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>217.53</c:v>
+                  <c:v>190.44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>289.44</c:v>
+                  <c:v>251.62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>332.43</c:v>
+                  <c:v>287.89</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>350.39</c:v>
+                  <c:v>282.52</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>368.79</c:v>
+                  <c:v>317.37</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>523.46</c:v>
+                  <c:v>394</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>475.01</c:v>
+                  <c:v>405.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4610,31 +4635,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>51.35</c:v>
+                  <c:v>44.76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67.06</c:v>
+                  <c:v>64.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.24</c:v>
+                  <c:v>75.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.33</c:v>
+                  <c:v>92.78</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>128.13</c:v>
+                  <c:v>114.59</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>149.41999999999999</c:v>
+                  <c:v>120.79</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>165.35</c:v>
+                  <c:v>136.43</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>194.97</c:v>
+                  <c:v>151.74</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>197.98</c:v>
+                  <c:v>182.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4915,9 +4940,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11744523660761895"/>
-          <c:y val="0.1086587733111383"/>
-          <c:w val="0.2486101663462332"/>
+          <c:x val="0.13951558938424077"/>
+          <c:y val="0.1118787167340026"/>
+          <c:w val="0.46152401638786217"/>
           <c:h val="0.31895746884143572"/>
         </c:manualLayout>
       </c:layout>
@@ -11550,16 +11575,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>33339</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11706,15 +11731,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:F8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Benchmark" dataDxfId="7"/>
-    <tableColumn id="2" name="Mean (ns)" dataDxfId="6"/>
-    <tableColumn id="3" name="Ratio" dataDxfId="5"/>
-    <tableColumn id="4" name="Rank" dataDxfId="4"/>
-    <tableColumn id="5" name="Gen 0" dataDxfId="3"/>
-    <tableColumn id="6" name="Allocated Bytes" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Benchmark" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mean (ns)" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ratio" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Rank" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Gen 0" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Allocated Bytes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12016,7 +12041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12298,7 +12323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Q8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -12695,7 +12720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -12880,11 +12905,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC17" sqref="AC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12893,7 +12918,7 @@
     <col min="2" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="14">
         <v>2</v>
       </c>
@@ -12921,239 +12946,288 @@
       <c r="J1" s="14">
         <v>10</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="16">
-        <v>35.18</v>
+        <v>30.31</v>
       </c>
       <c r="C2" s="16">
-        <v>48.49</v>
+        <v>43.51</v>
       </c>
       <c r="D2" s="16">
-        <v>63.77</v>
+        <v>63.08</v>
       </c>
       <c r="E2" s="16">
-        <v>100.7</v>
+        <v>90.85</v>
       </c>
       <c r="F2" s="16">
-        <v>116.58</v>
+        <v>103.37</v>
       </c>
       <c r="G2" s="16">
-        <v>147.13999999999999</v>
+        <v>123.32</v>
       </c>
       <c r="H2" s="16">
-        <v>188</v>
+        <v>135.19</v>
       </c>
       <c r="I2" s="16">
-        <v>201.92</v>
+        <v>148.81</v>
       </c>
       <c r="J2" s="16">
-        <v>202.92</v>
+        <v>181.85</v>
+      </c>
+      <c r="K2" s="16">
+        <v>0.27060000000000001</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="16">
-        <v>36.770000000000003</v>
+        <v>31.97</v>
       </c>
       <c r="C3" s="16">
-        <v>79.45</v>
+        <v>68.36</v>
       </c>
       <c r="D3" s="16">
-        <v>130.53</v>
+        <v>124.42</v>
       </c>
       <c r="E3" s="16">
-        <v>190.99</v>
+        <v>165.77</v>
       </c>
       <c r="F3" s="16">
-        <v>256.54000000000002</v>
+        <v>238.82</v>
       </c>
       <c r="G3" s="16">
-        <v>358.8</v>
+        <v>331.89</v>
       </c>
       <c r="H3" s="16">
-        <v>488.48</v>
+        <v>384.8</v>
       </c>
       <c r="I3" s="16">
-        <v>559.79999999999995</v>
+        <v>464.51</v>
       </c>
       <c r="J3" s="16">
-        <v>651.79</v>
+        <v>550.91</v>
+      </c>
+      <c r="K3" s="16">
+        <v>1.3513999999999999</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="16">
-        <v>37.15</v>
+        <v>30.14</v>
       </c>
       <c r="C4" s="16">
-        <v>48.36</v>
+        <v>42.61</v>
       </c>
       <c r="D4" s="16">
-        <v>62.73</v>
+        <v>60.26</v>
       </c>
       <c r="E4" s="16">
-        <v>81.739999999999995</v>
+        <v>74.87</v>
       </c>
       <c r="F4" s="16">
-        <v>100.52</v>
+        <v>92.47</v>
       </c>
       <c r="G4" s="16">
-        <v>121.92</v>
+        <v>105.45</v>
       </c>
       <c r="H4" s="16">
-        <v>137</v>
+        <v>113.45</v>
       </c>
       <c r="I4" s="16">
-        <v>171.35</v>
+        <v>125.57</v>
       </c>
       <c r="J4" s="16">
-        <v>177.58</v>
+        <v>154.71</v>
+      </c>
+      <c r="K4" s="16">
+        <v>0.24579999999999999</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="16">
-        <v>36.89</v>
+        <v>31.92</v>
       </c>
       <c r="C5" s="16">
-        <v>80.849999999999994</v>
+        <v>68.67</v>
       </c>
       <c r="D5" s="16">
-        <v>129.88999999999999</v>
+        <v>117.01</v>
       </c>
       <c r="E5" s="16">
-        <v>212.4</v>
+        <v>171.78</v>
       </c>
       <c r="F5" s="16">
-        <v>324.85000000000002</v>
+        <v>228.46</v>
       </c>
       <c r="G5" s="16">
-        <v>400.4</v>
+        <v>295.26</v>
       </c>
       <c r="H5" s="16">
-        <v>448.09</v>
+        <v>373.92</v>
       </c>
       <c r="I5" s="16">
-        <v>657.48</v>
+        <v>457.44</v>
       </c>
       <c r="J5" s="16">
-        <v>700.75</v>
+        <v>564.54999999999995</v>
+      </c>
+      <c r="K5" s="16">
+        <v>1.3513999999999999</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="16">
-        <v>133.80000000000001</v>
+      <c r="B6" s="4">
+        <v>116.05</v>
       </c>
       <c r="C6" s="16">
-        <v>191.67</v>
+        <v>167.63</v>
       </c>
       <c r="D6" s="16">
-        <v>212.86</v>
+        <v>203.84</v>
       </c>
       <c r="E6" s="16">
-        <v>285.92</v>
+        <v>255.88</v>
       </c>
       <c r="F6" s="16">
-        <v>326.55</v>
+        <v>273.02</v>
       </c>
       <c r="G6" s="16">
-        <v>350.79</v>
+        <v>284.45999999999998</v>
       </c>
       <c r="H6" s="16">
-        <v>366.17</v>
+        <v>303.91000000000003</v>
       </c>
       <c r="I6" s="16">
-        <v>504.34</v>
+        <v>386.91</v>
       </c>
       <c r="J6" s="16">
-        <v>464.81</v>
+        <v>405.28</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0.7319</v>
+      </c>
+      <c r="L6" s="37" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="16">
-        <v>132.9</v>
+        <v>116.51</v>
       </c>
       <c r="C7" s="16">
-        <v>193.09</v>
+        <v>166.51</v>
       </c>
       <c r="D7" s="16">
-        <v>217.53</v>
+        <v>190.44</v>
       </c>
       <c r="E7" s="16">
-        <v>289.44</v>
+        <v>251.62</v>
       </c>
       <c r="F7" s="16">
-        <v>332.43</v>
+        <v>287.89</v>
       </c>
       <c r="G7" s="16">
-        <v>350.39</v>
+        <v>282.52</v>
       </c>
       <c r="H7" s="16">
-        <v>368.79</v>
+        <v>317.37</v>
       </c>
       <c r="I7" s="16">
-        <v>523.46</v>
+        <v>394</v>
       </c>
       <c r="J7" s="16">
-        <v>475.01</v>
+        <v>405.89</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0.7319</v>
+      </c>
+      <c r="L7" s="37" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="16">
-        <v>51.35</v>
+        <v>44.76</v>
       </c>
       <c r="C8" s="16">
-        <v>67.06</v>
+        <v>64.45</v>
       </c>
       <c r="D8" s="16">
-        <v>88.24</v>
+        <v>75.22</v>
       </c>
       <c r="E8" s="16">
-        <v>100.33</v>
+        <v>92.78</v>
       </c>
       <c r="F8" s="16">
-        <v>128.13</v>
+        <v>114.59</v>
       </c>
       <c r="G8" s="16">
-        <v>149.41999999999999</v>
+        <v>120.79</v>
       </c>
       <c r="H8" s="16">
-        <v>165.35</v>
+        <v>136.43</v>
       </c>
       <c r="I8" s="16">
-        <v>194.97</v>
+        <v>151.74</v>
       </c>
       <c r="J8" s="16">
-        <v>197.98</v>
+        <v>182.27</v>
+      </c>
+      <c r="K8" s="16">
+        <v>0.24959999999999999</v>
+      </c>
+      <c r="L8" s="37" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13599,7 +13673,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13786,10 +13860,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add StringBuilderCached class and Benchmark
</commit_message>
<xml_diff>
--- a/ArrayVsDictionaryBenchmark.xlsx
+++ b/ArrayVsDictionaryBenchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivk\source\repos\matlus\VariousBenchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FF1ED4-868E-4C6E-9250-A7A01052BA8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43ADC418-DDA3-4AC2-BF46-805354920675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="285" windowWidth="28095" windowHeight="14865" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VaueType Array-Dictionary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
     <t>Sorted Array</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>1048 B</t>
+  </si>
+  <si>
+    <t>StringBuilderLoopCached</t>
+  </si>
+  <si>
+    <t>3104 B</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -547,6 +553,10 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="4" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -3935,15 +3945,78 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="7"/>
           <c:order val="0"/>
           <c:tx>
+            <c:v>PlusOperator</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'String Concatention'!$B$2:$J$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>30.31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>103.37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>123.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>135.19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>148.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>181.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D2D2-4502-AE18-9D2F1784EE88}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
             <c:strRef>
-              <c:f>'String Concatention'!$A$2</c:f>
+              <c:f>'String Concatention'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PlusOperator</c:v>
+                  <c:v>PlusOperatorLoop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3998,36 +4071,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'String Concatention'!$B$2:$J$2</c:f>
+              <c:f>'String Concatention'!$B$3:$J$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>30.31</c:v>
+                  <c:v>31.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.51</c:v>
+                  <c:v>68.36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.08</c:v>
+                  <c:v>124.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.85</c:v>
+                  <c:v>165.77</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.37</c:v>
+                  <c:v>238.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>123.32</c:v>
+                  <c:v>331.89</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>135.19</c:v>
+                  <c:v>384.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>148.81</c:v>
+                  <c:v>464.51</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>181.85</c:v>
+                  <c:v>550.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4041,14 +4114,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'String Concatention'!$A$3</c:f>
+              <c:f>'String Concatention'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PlusOperatorLoop</c:v>
+                  <c:v>ConcatMethod</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4103,36 +4176,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'String Concatention'!$B$3:$J$3</c:f>
+              <c:f>'String Concatention'!$B$4:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>31.97</c:v>
+                  <c:v>30.14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.36</c:v>
+                  <c:v>42.61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>124.42</c:v>
+                  <c:v>60.26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>165.77</c:v>
+                  <c:v>74.87</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>238.82</c:v>
+                  <c:v>92.47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>331.89</c:v>
+                  <c:v>105.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>384.8</c:v>
+                  <c:v>113.45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>464.51</c:v>
+                  <c:v>125.57</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>550.91</c:v>
+                  <c:v>154.71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4146,14 +4219,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'String Concatention'!$A$4</c:f>
+              <c:f>'String Concatention'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ConcatMethod</c:v>
+                  <c:v>ConcatLoop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4208,36 +4281,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'String Concatention'!$B$4:$J$4</c:f>
+              <c:f>'String Concatention'!$B$5:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>30.14</c:v>
+                  <c:v>31.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.61</c:v>
+                  <c:v>68.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.26</c:v>
+                  <c:v>117.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.87</c:v>
+                  <c:v>171.78</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92.47</c:v>
+                  <c:v>228.46</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105.45</c:v>
+                  <c:v>295.26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>113.45</c:v>
+                  <c:v>373.92</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>125.57</c:v>
+                  <c:v>457.44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>154.71</c:v>
+                  <c:v>564.54999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4251,14 +4324,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'String Concatention'!$A$5</c:f>
+              <c:f>'String Concatention'!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ConcatLoop</c:v>
+                  <c:v>StringBuilder</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4313,36 +4386,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'String Concatention'!$B$5:$J$5</c:f>
+              <c:f>'String Concatention'!$B$6:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>31.92</c:v>
+                  <c:v>116.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.67</c:v>
+                  <c:v>167.63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117.01</c:v>
+                  <c:v>203.84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>171.78</c:v>
+                  <c:v>255.88</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>228.46</c:v>
+                  <c:v>273.02</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>295.26</c:v>
+                  <c:v>284.45999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>373.92</c:v>
+                  <c:v>303.91000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>457.44</c:v>
+                  <c:v>386.91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>564.54999999999995</c:v>
+                  <c:v>405.28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4356,14 +4429,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'String Concatention'!$A$6</c:f>
+              <c:f>'String Concatention'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>StringBuilder</c:v>
+                  <c:v>StringBuilderLoop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4418,36 +4491,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'String Concatention'!$B$6:$J$6</c:f>
+              <c:f>'String Concatention'!$B$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>116.05</c:v>
+                  <c:v>116.51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>167.63</c:v>
+                  <c:v>166.51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>203.84</c:v>
+                  <c:v>190.44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>255.88</c:v>
+                  <c:v>251.62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>273.02</c:v>
+                  <c:v>287.89</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>284.45999999999998</c:v>
+                  <c:v>282.52</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>303.91000000000003</c:v>
+                  <c:v>317.37</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>386.91</c:v>
+                  <c:v>394</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>405.28</c:v>
+                  <c:v>405.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4456,111 +4529,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-E58F-41BF-BC86-7F82CCE41C29}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'String Concatention'!$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>StringBuilderLoop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'String Concatention'!$B$1:$J$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'String Concatention'!$B$7:$J$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>116.51</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>166.51</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>190.44</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>251.62</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>287.89</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>282.52</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>317.37</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>394</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>405.89</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-E58F-41BF-BC86-7F82CCE41C29}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4573,7 +4541,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>StringJoin</c:v>
+                  <c:v>StringBuilderLoopCached</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4635,31 +4603,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>44.76</c:v>
+                  <c:v>55.74</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.45</c:v>
+                  <c:v>69.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.22</c:v>
+                  <c:v>140.66999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92.78</c:v>
+                  <c:v>161.49</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>114.59</c:v>
+                  <c:v>164.36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120.79</c:v>
+                  <c:v>215.35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>136.43</c:v>
+                  <c:v>245.16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>151.74</c:v>
+                  <c:v>272.33999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>182.27</c:v>
+                  <c:v>306.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4668,6 +4636,111 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-E58F-41BF-BC86-7F82CCE41C29}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'String Concatention'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StringJoin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'String Concatention'!$B$1:$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'String Concatention'!$B$9:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>44.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75.22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120.79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136.43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>151.74</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>182.27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E58F-41BF-BC86-7F82CCE41C29}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4942,8 +5015,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.13951558938424077"/>
           <c:y val="0.1118787167340026"/>
-          <c:w val="0.46152401638786217"/>
-          <c:h val="0.31895746884143572"/>
+          <c:w val="0.65009326664355638"/>
+          <c:h val="5.6246328205615537E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -12906,15 +12979,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC17" sqref="AC17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
@@ -13181,41 +13254,79 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="4">
+        <v>55.74</v>
+      </c>
+      <c r="C8" s="4">
+        <v>69.08</v>
+      </c>
+      <c r="D8" s="4">
+        <v>140.66999999999999</v>
+      </c>
+      <c r="E8" s="4">
+        <v>161.49</v>
+      </c>
+      <c r="F8" s="4">
+        <v>164.36</v>
+      </c>
+      <c r="G8" s="4">
+        <v>215.35</v>
+      </c>
+      <c r="H8" s="4">
+        <v>245.16</v>
+      </c>
+      <c r="I8" s="4">
+        <v>272.33999999999997</v>
+      </c>
+      <c r="J8" s="4">
+        <v>306.39</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.73960000000000004</v>
+      </c>
+      <c r="L8" s="39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B9" s="16">
         <v>44.76</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C9" s="16">
         <v>64.45</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D9" s="16">
         <v>75.22</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E9" s="16">
         <v>92.78</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F9" s="16">
         <v>114.59</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G9" s="16">
         <v>120.79</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H9" s="16">
         <v>136.43</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I9" s="16">
         <v>151.74</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J9" s="16">
         <v>182.27</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K9" s="16">
         <v>0.24959999999999999</v>
       </c>
-      <c r="L8" s="37" t="s">
+      <c r="L9" s="37" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added For Loop benchmark
</commit_message>
<xml_diff>
--- a/ArrayVsDictionaryBenchmark.xlsx
+++ b/ArrayVsDictionaryBenchmark.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivk\source\repos\matlus\VariousBenchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43ADC418-DDA3-4AC2-BF46-805354920675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEAB16C-D323-4D85-BFF4-B8DF6824454C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="285" windowWidth="28095" windowHeight="14865" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="1710" windowWidth="28005" windowHeight="15345" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VaueType Array-Dictionary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>Sorted Array</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>3104 B</t>
+  </si>
+  <si>
+    <t>GetUsingMergeSetsAndSingleToUpper</t>
+  </si>
+  <si>
+    <t>GetWithoutLINQNoToUpperForLoop</t>
   </si>
 </sst>
 </file>
@@ -7707,6 +7713,757 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>To LINQ or Not to LINQ</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LinqWhere!$A$2:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>GetUsingMultipleToUpper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>579.90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>LinqWhere!$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>579.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-6B72-42DA-AD77-6B005492BD28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LinqWhere!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GetUsingMultipleEqualityComparer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>LinqWhere!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1000.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-6B72-42DA-AD77-6B005492BD28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LinqWhere!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GetUsingMergeSetsAndSingleToUpper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>LinqWhere!$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>624.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-6B72-42DA-AD77-6B005492BD28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LinqWhere!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GetUsingConcatAndMultipleToUpper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>LinqWhere!$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1928.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-6B72-42DA-AD77-6B005492BD28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LinqWhere!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GetUsingQueryExpLetAndOneToUpper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>LinqWhere!$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>691.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-6B72-42DA-AD77-6B005492BD28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LinqWhere!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GetUsingLocalvariableAssignmentForToUpper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>LinqWhere!$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>431.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-6B72-42DA-AD77-6B005492BD28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LinqWhere!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GetWithoutLINQ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>LinqWhere!$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>288.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-6B72-42DA-AD77-6B005492BD28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LinqWhere!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GetWithoutLINQNoToUpper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>LinqWhere!$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>206</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-6B72-42DA-AD77-6B005492BD28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LinqWhere!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GetWithoutLINQNoToUpperForLoop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>LinqWhere!$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>165.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-6B72-42DA-AD77-6B005492BD28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="589354480"/>
+        <c:axId val="589354152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="589354480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="589354152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="589354152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in Nano Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="589354480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7987,6 +8744,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -11020,6 +11817,509 @@
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -11803,9 +13103,50 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{769F6578-50E1-445B-A7A7-B64FF9A328B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Benchmark" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mean (ns)" dataDxfId="4"/>
@@ -12981,7 +14322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -13788,7 +15129,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13972,10 +15313,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -14012,19 +15353,19 @@
         <v>45</v>
       </c>
       <c r="B2" s="5">
-        <v>1142.5</v>
+        <v>579.9</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="4">
-        <v>8.0100000000000005E-2</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="F2" s="4">
-        <v>256</v>
+        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -14032,126 +15373,167 @@
         <v>46</v>
       </c>
       <c r="B3" s="4">
-        <v>890.7</v>
+        <v>1000.1</v>
       </c>
       <c r="C3" s="4">
-        <v>0.78</v>
+        <v>1.72</v>
       </c>
       <c r="D3" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4">
-        <v>8.9599999999999999E-2</v>
+        <v>0.1144</v>
       </c>
       <c r="F3" s="4">
-        <v>284</v>
+        <v>488</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B4" s="5">
-        <v>1884.4</v>
+        <v>624.6</v>
       </c>
       <c r="C4" s="4">
-        <v>1.65</v>
+        <v>1.08</v>
       </c>
       <c r="D4" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="4">
-        <v>0.18310000000000001</v>
+        <v>9.06E-2</v>
       </c>
       <c r="F4" s="4">
-        <v>585</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="4">
-        <v>828.8</v>
+        <v>47</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1928.1</v>
       </c>
       <c r="C5" s="4">
-        <v>0.73</v>
+        <v>3.32</v>
       </c>
       <c r="D5" s="4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E5" s="4">
-        <v>9.35E-2</v>
+        <v>0.2213</v>
       </c>
       <c r="F5" s="4">
-        <v>296</v>
+        <v>944</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="4">
-        <v>689.6</v>
+        <v>691.9</v>
       </c>
       <c r="C6" s="4">
-        <v>0.61</v>
+        <v>1.19</v>
       </c>
       <c r="D6" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E6" s="4">
-        <v>5.5300000000000002E-2</v>
+        <v>0.123</v>
       </c>
       <c r="F6" s="4">
-        <v>176</v>
+        <v>520</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="4">
-        <v>564.6</v>
+        <v>431.2</v>
       </c>
       <c r="C7" s="4">
-        <v>0.49</v>
+        <v>0.74</v>
       </c>
       <c r="D7" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" s="4">
-        <v>3.5299999999999998E-2</v>
+        <v>7.2499999999999995E-2</v>
       </c>
       <c r="F7" s="4">
-        <v>112</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="4">
+        <v>288.2</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4.53E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="4">
-        <v>186.5</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.16</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="B9" s="4">
+        <v>206</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.36</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="F9" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="4">
+        <v>165.1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="4">
-        <v>1.6500000000000001E-2</v>
-      </c>
-      <c r="F8" s="4">
-        <v>52</v>
+      <c r="E10" s="4">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added additional benchmarks and added graphs in the Excel spreadsheet
</commit_message>
<xml_diff>
--- a/ArrayVsDictionaryBenchmark.xlsx
+++ b/ArrayVsDictionaryBenchmark.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivk\source\repos\matlus\VariousBenchmarks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\VariousBenchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEAB16C-D323-4D85-BFF4-B8DF6824454C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6853CE-A59B-4046-93C7-AAB71F8A194A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="1710" windowWidth="28005" windowHeight="15345" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VaueType Array-Dictionary" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="TableValuedParameters" sheetId="4" r:id="rId5"/>
     <sheet name="SlugProducer" sheetId="6" r:id="rId6"/>
     <sheet name="LinqWhere" sheetId="7" r:id="rId7"/>
+    <sheet name="BrnachPrediction" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>Sorted Array</t>
   </si>
@@ -184,12 +185,6 @@
     <t>GetUsingLocalvariableAssignmentForToUpper</t>
   </si>
   <si>
-    <t>GetWithoutLINQ</t>
-  </si>
-  <si>
-    <t>GetWithoutLINQNoToUpper</t>
-  </si>
-  <si>
     <t>Ratio</t>
   </si>
   <si>
@@ -239,6 +234,24 @@
   </si>
   <si>
     <t>GetWithoutLINQNoToUpperForLoop</t>
+  </si>
+  <si>
+    <t>GetWithoutLINQNoToUpperForEach</t>
+  </si>
+  <si>
+    <t>GetWithoutLINQForEach</t>
+  </si>
+  <si>
+    <t>GetWithoutLINQForLoop</t>
+  </si>
+  <si>
+    <t>IterateOverOrderedArray</t>
+  </si>
+  <si>
+    <t>IterateOverRandomOrderedArray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RandomOrderedArrayLinqWhere </t>
   </si>
 </sst>
 </file>
@@ -571,7 +584,151 @@
     <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -7748,7 +7905,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>To LINQ or Not to LINQ</a:t>
+              <a:t>To LINQ or Not to LINQ; That is the question</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7801,7 +7958,7 @@
                   <c:v>GetUsingMultipleToUpper</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>579.90</c:v>
+                  <c:v>706.40</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7816,6 +7973,14 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Varios Options</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>LinqWhere!$B$2</c:f>
@@ -7823,7 +7988,7 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>579.9</c:v>
+                  <c:v>706.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7858,14 +8023,22 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Varios Options</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>LinqWhere!$B$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1000.1</c:v>
+                  <c:v>1183.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7900,6 +8073,14 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Varios Options</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>LinqWhere!$B$4</c:f>
@@ -7907,7 +8088,7 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>624.6</c:v>
+                  <c:v>597.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7942,6 +8123,14 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Varios Options</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>LinqWhere!$B$5</c:f>
@@ -7949,7 +8138,7 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1928.1</c:v>
+                  <c:v>2649.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7984,6 +8173,14 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Varios Options</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>LinqWhere!$B$6</c:f>
@@ -7991,7 +8188,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>691.9</c:v>
+                  <c:v>601.29999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8026,6 +8223,14 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Varios Options</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>LinqWhere!$B$7</c:f>
@@ -8033,7 +8238,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>431.2</c:v>
+                  <c:v>390.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8053,7 +8258,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GetWithoutLINQ</c:v>
+                  <c:v>GetWithoutLINQForEach</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8070,6 +8275,14 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Varios Options</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>LinqWhere!$B$8</c:f>
@@ -8077,7 +8290,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>288.2</c:v>
+                  <c:v>430.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8089,7 +8302,7 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="7"/>
+          <c:idx val="9"/>
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
@@ -8097,7 +8310,59 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GetWithoutLINQNoToUpper</c:v>
+                  <c:v>GetWithoutLINQForLoop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Varios Options</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LinqWhere!$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>341.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6FA0-42EB-9CBB-965F6192F84B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LinqWhere!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GetWithoutLINQNoToUpperForEach</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8114,14 +8379,22 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Varios Options</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LinqWhere!$B$9</c:f>
+              <c:f>LinqWhere!$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>206</c:v>
+                  <c:v>213.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8134,10 +8407,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
-          <c:order val="8"/>
+          <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>LinqWhere!$A$10</c:f>
+              <c:f>LinqWhere!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8158,14 +8431,22 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Varios Options</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LinqWhere!$B$10</c:f>
+              <c:f>LinqWhere!$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>165.1</c:v>
+                  <c:v>131.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8226,7 +8507,534 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="589354152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="589354152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in Nano Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="589354480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Branch Prediction</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BrnachPrediction!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IterateOverOrderedArray</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>BrnachPrediction!$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>476.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-CCFF-4DF0-945D-1256009D3D56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BrnachPrediction!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IterateOverRandomOrderedArray</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>BrnachPrediction!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3729</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-CCFF-4DF0-945D-1256009D3D56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BrnachPrediction!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RandomOrderedArrayLinqWhere </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>BrnachPrediction!$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8154.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-CCFF-4DF0-945D-1256009D3D56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="589354480"/>
+        <c:axId val="589354152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="589354480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Benchmarks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8784,6 +9592,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -12319,6 +13167,509 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13113,9 +14464,9 @@
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>618112</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -13144,16 +14495,74 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>33338</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8113E46A-CF3B-4ECC-BC70-3A2205274540}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Benchmark" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mean (ns)" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ratio" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Rank" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Gen 0" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Allocated Bytes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Benchmark" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mean (ns)" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ratio" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Rank" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Gen 0" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Allocated Bytes" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{78C68ADC-C263-48F5-9DB4-8F3840CCC8EF}" name="Table15" displayName="Table15" ref="A1:F4" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F4" xr:uid="{44C6E141-2C16-4362-B65D-C9CD8D3E4916}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{CBFDE53B-F40A-45AA-94F9-2A4CE5A40CE7}" name="Benchmark" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{5CD17E29-93E0-41A7-9B8C-1BABD405593F}" name="Mean (ns)" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{AAB2AB74-394D-4DCF-AC82-1874B2B4F1A0}" name="Ratio" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{51783A2E-27C0-4145-B6B7-10BF1F255DD9}" name="Rank" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{86B86C85-2922-4873-B5AD-601831D88823}" name="Gen 0" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{9771DE3E-8973-485C-8227-F64293B18C14}" name="Allocated Bytes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13462,13 +14871,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="25.53125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.19921875" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B2" s="23">
         <v>5</v>
       </c>
@@ -13518,7 +14927,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
@@ -13571,7 +14980,7 @@
         <v>4024.3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="24" t="s">
         <v>4</v>
       </c>
@@ -13624,7 +15033,7 @@
         <v>2303.1999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
@@ -13677,7 +15086,7 @@
         <v>962.1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A6" s="24" t="s">
         <v>2</v>
       </c>
@@ -13744,22 +15153,22 @@
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="16.5" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="9.140625" style="4"/>
-    <col min="10" max="10" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="31.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="9.19921875" style="4"/>
+    <col min="10" max="10" width="9.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.53125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.73046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.73046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.53125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.19921875" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B2" s="1">
         <v>5</v>
       </c>
@@ -13809,7 +15218,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -13862,7 +15271,7 @@
         <v>20544.34</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -13915,7 +15324,7 @@
         <v>54899.68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -13968,7 +15377,7 @@
         <v>23633.95</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -14021,7 +15430,7 @@
         <v>72404.929999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -14074,7 +15483,7 @@
         <v>25939.16</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -14138,19 +15547,19 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="34"/>
-    <col min="10" max="10" width="9.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="34"/>
+    <col min="2" max="5" width="11.265625" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.19921875" style="34"/>
+    <col min="10" max="10" width="9.46484375" style="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.19921875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
@@ -14173,7 +15582,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A2" s="35" t="s">
         <v>9</v>
       </c>
@@ -14196,7 +15605,7 @@
         <v>1.5389999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="35" t="s">
         <v>10</v>
       </c>
@@ -14220,7 +15629,7 @@
       </c>
       <c r="H3" s="36"/>
     </row>
-    <row r="4" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="35" t="s">
         <v>11</v>
       </c>
@@ -14243,7 +15652,7 @@
         <v>12.465</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A5" s="35" t="s">
         <v>12</v>
       </c>
@@ -14266,7 +15675,7 @@
         <v>12.762</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A6" s="35" t="s">
         <v>13</v>
       </c>
@@ -14289,7 +15698,7 @@
         <v>2.052</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A7" s="35" t="s">
         <v>14</v>
       </c>
@@ -14326,13 +15735,13 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="27.46484375" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.19921875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B1" s="14">
         <v>2</v>
       </c>
@@ -14361,13 +15770,13 @@
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -14402,10 +15811,10 @@
         <v>0.27060000000000001</v>
       </c>
       <c r="L2" s="37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
@@ -14440,10 +15849,10 @@
         <v>1.3513999999999999</v>
       </c>
       <c r="L3" s="37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
@@ -14478,10 +15887,10 @@
         <v>0.24579999999999999</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
@@ -14516,10 +15925,10 @@
         <v>1.3513999999999999</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A6" s="15" t="s">
         <v>24</v>
       </c>
@@ -14554,10 +15963,10 @@
         <v>0.7319</v>
       </c>
       <c r="L6" s="37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
@@ -14592,12 +16001,12 @@
         <v>0.7319</v>
       </c>
       <c r="L7" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A8" s="38" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
-        <v>65</v>
       </c>
       <c r="B8" s="4">
         <v>55.74</v>
@@ -14630,10 +16039,10 @@
         <v>0.73960000000000004</v>
       </c>
       <c r="L8" s="39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A9" s="15" t="s">
         <v>26</v>
       </c>
@@ -14668,7 +16077,7 @@
         <v>0.24959999999999999</v>
       </c>
       <c r="L9" s="37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -14686,15 +16095,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="22" width="9.140625" style="9"/>
-    <col min="23" max="23" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="31.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="22" width="9.19921875" style="9"/>
+    <col min="23" max="23" width="11.265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.19921875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A1" s="10"/>
       <c r="B1" s="10">
         <v>5</v>
@@ -14763,7 +16172,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
@@ -14834,7 +16243,7 @@
         <v>47361.822999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
@@ -14905,7 +16314,7 @@
         <v>46784.144999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
@@ -14976,7 +16385,7 @@
         <v>47061.86</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
@@ -15047,7 +16456,7 @@
         <v>106204.17</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
@@ -15129,24 +16538,24 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="17"/>
-    <col min="10" max="10" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="96.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="17"/>
+    <col min="3" max="3" width="13.53125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.46484375" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.53125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.46484375" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.19921875" style="17"/>
+    <col min="10" max="10" width="13.53125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="96.53125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.19921875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B1" s="18" t="s">
         <v>31</v>
       </c>
@@ -15169,7 +16578,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A2" s="19" t="s">
         <v>27</v>
       </c>
@@ -15195,7 +16604,7 @@
         <v>960.3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="19" t="s">
         <v>28</v>
       </c>
@@ -15221,7 +16630,7 @@
         <v>1663.2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="19" t="s">
         <v>29</v>
       </c>
@@ -15247,7 +16656,7 @@
         <v>777.4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="J7" s="18" t="s">
         <v>31</v>
       </c>
@@ -15255,7 +16664,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="J8" s="18" t="s">
         <v>32</v>
       </c>
@@ -15263,7 +16672,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="J9" s="18" t="s">
         <v>37</v>
       </c>
@@ -15271,7 +16680,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="J10" s="18" t="s">
         <v>36</v>
       </c>
@@ -15279,7 +16688,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="J11" s="18" t="s">
         <v>35</v>
       </c>
@@ -15287,7 +16696,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="J12" s="18" t="s">
         <v>34</v>
       </c>
@@ -15295,7 +16704,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="J13" s="18" t="s">
         <v>33</v>
       </c>
@@ -15303,7 +16712,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -15313,219 +16722,239 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="16.5" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="42.53125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.53125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.19921875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.19921875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="C1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="5">
-        <v>579.9</v>
+        <v>706.4</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4">
-        <v>0.10299999999999999</v>
+        <v>8.1100000000000005E-2</v>
       </c>
       <c r="F2" s="4">
-        <v>432</v>
+        <v>680</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="4">
-        <v>1000.1</v>
+      <c r="B3" s="5">
+        <v>1183.2</v>
       </c>
       <c r="C3" s="4">
-        <v>1.72</v>
+        <v>1.67</v>
       </c>
       <c r="D3" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="4">
-        <v>0.1144</v>
+        <v>9.5399999999999999E-2</v>
       </c>
       <c r="F3" s="4">
-        <v>488</v>
+        <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A4" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="5">
-        <v>624.6</v>
+        <v>597.9</v>
       </c>
       <c r="C4" s="4">
-        <v>1.08</v>
+        <v>0.84</v>
       </c>
       <c r="D4" s="4">
         <v>6</v>
       </c>
       <c r="E4" s="4">
-        <v>9.06E-2</v>
+        <v>5.6300000000000003E-2</v>
       </c>
       <c r="F4" s="4">
-        <v>384</v>
+        <v>472</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="5">
-        <v>1928.1</v>
+        <v>2649.2</v>
       </c>
       <c r="C5" s="4">
-        <v>3.32</v>
+        <v>3.74</v>
       </c>
       <c r="D5" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="4">
-        <v>0.2213</v>
+        <v>0.20219999999999999</v>
       </c>
       <c r="F5" s="4">
-        <v>944</v>
+        <v>1712</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A6" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="4">
-        <v>691.9</v>
+        <v>601.29999999999995</v>
       </c>
       <c r="C6" s="4">
-        <v>1.19</v>
+        <v>0.85</v>
       </c>
       <c r="D6" s="4">
         <v>7</v>
       </c>
       <c r="E6" s="4">
-        <v>0.123</v>
+        <v>8.3900000000000002E-2</v>
       </c>
       <c r="F6" s="4">
-        <v>520</v>
+        <v>704</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="4">
-        <v>431.2</v>
+        <v>390.1</v>
       </c>
       <c r="C7" s="4">
-        <v>0.74</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D7" s="4">
         <v>4</v>
       </c>
       <c r="E7" s="4">
-        <v>7.2499999999999995E-2</v>
+        <v>4.6699999999999998E-2</v>
       </c>
       <c r="F7" s="4">
-        <v>304</v>
+        <v>392</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B8" s="4">
-        <v>288.2</v>
+        <v>430.6</v>
       </c>
       <c r="C8" s="4">
-        <v>0.5</v>
+        <v>0.61</v>
       </c>
       <c r="D8" s="4">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.6">
+      <c r="A9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="4">
+        <v>341.1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.48</v>
+      </c>
+      <c r="D9" s="4">
         <v>3</v>
       </c>
-      <c r="E8" s="4">
-        <v>4.53E-2</v>
-      </c>
-      <c r="F8" s="4">
-        <v>192</v>
+      <c r="E9" s="4">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="F9" s="4">
+        <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="4">
-        <v>206</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.36</v>
-      </c>
-      <c r="D9" s="4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.6">
+      <c r="A10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="4">
+        <v>213.1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="4">
         <v>2</v>
       </c>
-      <c r="E9" s="4">
-        <v>1.8800000000000001E-2</v>
-      </c>
-      <c r="F9" s="4">
-        <v>80</v>
+      <c r="E10" s="4">
+        <v>8.6E-3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="4">
-        <v>165.1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="D10" s="4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.6">
+      <c r="A11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="4">
+        <v>131.5</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="D11" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="4">
-        <v>9.2999999999999992E-3</v>
-      </c>
-      <c r="F10" s="4">
-        <v>40</v>
+      <c r="E11" s="4">
+        <v>3.8E-3</v>
+      </c>
+      <c r="F11" s="4">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -15536,4 +16965,110 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C534E5F-56B3-464F-ACD4-646EB824795D}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="16.5" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="1" max="1" width="42.53125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.53125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.19921875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.19921875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
+      <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
+      <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="5">
+        <v>476.4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
+      <c r="A3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3729</v>
+      </c>
+      <c r="C3" s="4">
+        <v>7.83</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
+      <c r="A4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="5">
+        <v>8154.7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>17.14</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated graphs and added one more bench mark for the branch prediction code
</commit_message>
<xml_diff>
--- a/ArrayVsDictionaryBenchmark.xlsx
+++ b/ArrayVsDictionaryBenchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\VariousBenchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6853CE-A59B-4046-93C7-AAB71F8A194A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9515C4-547C-4C75-AFB7-DEB6544F61BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9440" yWindow="370" windowWidth="28800" windowHeight="15830" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VaueType Array-Dictionary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t>Sorted Array</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t xml:space="preserve">RandomOrderedArrayLinqWhere </t>
+  </si>
+  <si>
+    <t>SortRandomOrderedArrayAndIterate</t>
   </si>
 </sst>
 </file>
@@ -8856,7 +8859,7 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>476.4</c:v>
+                  <c:v>470.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8902,7 +8905,7 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3729</c:v>
+                  <c:v>3561.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8948,7 +8951,7 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8154.7</c:v>
+                  <c:v>8413.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8956,6 +8959,48 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-CCFF-4DF0-945D-1256009D3D56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BrnachPrediction!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SortRandomOrderedArrayAndIterate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>BrnachPrediction!$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7741.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F6FF-4590-AD43-F8F9F206A88C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -14465,7 +14510,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>618112</xdr:colOff>
+      <xdr:colOff>6756</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -14554,8 +14599,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{78C68ADC-C263-48F5-9DB4-8F3840CCC8EF}" name="Table15" displayName="Table15" ref="A1:F4" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F4" xr:uid="{44C6E141-2C16-4362-B65D-C9CD8D3E4916}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{78C68ADC-C263-48F5-9DB4-8F3840CCC8EF}" name="Table15" displayName="Table15" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F5" xr:uid="{44C6E141-2C16-4362-B65D-C9CD8D3E4916}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CBFDE53B-F40A-45AA-94F9-2A4CE5A40CE7}" name="Benchmark" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{5CD17E29-93E0-41A7-9B8C-1BABD405593F}" name="Mean (ns)" dataDxfId="4"/>
@@ -14871,13 +14916,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.53125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.19921875" style="22"/>
+    <col min="1" max="1" width="25.54296875" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:17" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="23">
         <v>5</v>
       </c>
@@ -14927,7 +14972,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:17" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
@@ -14980,7 +15025,7 @@
         <v>4024.3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="24" t="s">
         <v>4</v>
       </c>
@@ -15033,7 +15078,7 @@
         <v>2303.1999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
@@ -15086,7 +15131,7 @@
         <v>962.1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="24" t="s">
         <v>2</v>
       </c>
@@ -15153,22 +15198,22 @@
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="16.5" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="9.19921875" style="4"/>
-    <col min="10" max="10" width="9.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.53125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.53125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.19921875" style="4"/>
+    <col min="1" max="1" width="31.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="9.1796875" style="4"/>
+    <col min="10" max="10" width="9.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:17" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="1">
         <v>5</v>
       </c>
@@ -15218,7 +15263,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:17" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -15271,7 +15316,7 @@
         <v>20544.34</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -15324,7 +15369,7 @@
         <v>54899.68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -15377,7 +15422,7 @@
         <v>23633.95</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -15430,7 +15475,7 @@
         <v>72404.929999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -15483,7 +15528,7 @@
         <v>25939.16</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -15550,16 +15595,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.265625" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.19921875" style="34"/>
-    <col min="10" max="10" width="9.46484375" style="34" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.19921875" style="34"/>
+    <col min="2" max="5" width="11.26953125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.1796875" style="34"/>
+    <col min="10" max="10" width="9.453125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
@@ -15582,7 +15627,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:8" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="35" t="s">
         <v>9</v>
       </c>
@@ -15605,7 +15650,7 @@
         <v>1.5389999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="35" t="s">
         <v>10</v>
       </c>
@@ -15629,7 +15674,7 @@
       </c>
       <c r="H3" s="36"/>
     </row>
-    <row r="4" spans="1:8" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="35" t="s">
         <v>11</v>
       </c>
@@ -15652,7 +15697,7 @@
         <v>12.465</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="35" t="s">
         <v>12</v>
       </c>
@@ -15675,7 +15720,7 @@
         <v>12.762</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="35" t="s">
         <v>13</v>
       </c>
@@ -15698,7 +15743,7 @@
         <v>2.052</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="35" t="s">
         <v>14</v>
       </c>
@@ -15735,13 +15780,13 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.46484375" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.19921875" style="13"/>
+    <col min="1" max="1" width="27.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:12" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B1" s="14">
         <v>2</v>
       </c>
@@ -15776,7 +15821,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:12" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -15814,7 +15859,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
@@ -15852,7 +15897,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
@@ -15890,7 +15935,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
@@ -15928,7 +15973,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="15" t="s">
         <v>24</v>
       </c>
@@ -15966,7 +16011,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
@@ -16004,7 +16049,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A8" s="38" t="s">
         <v>63</v>
       </c>
@@ -16042,7 +16087,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="15" t="s">
         <v>26</v>
       </c>
@@ -16095,15 +16140,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.53125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="22" width="9.19921875" style="9"/>
-    <col min="23" max="23" width="11.265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.19921875" style="9"/>
+    <col min="1" max="1" width="31.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="22" width="9.1796875" style="9"/>
+    <col min="23" max="23" width="11.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.1796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:23" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="10"/>
       <c r="B1" s="10">
         <v>5</v>
@@ -16172,7 +16217,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:23" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
@@ -16243,7 +16288,7 @@
         <v>47361.822999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
@@ -16314,7 +16359,7 @@
         <v>46784.144999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
@@ -16385,7 +16430,7 @@
         <v>47061.86</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
@@ -16456,7 +16501,7 @@
         <v>106204.17</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
@@ -16541,21 +16586,21 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.19921875" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.53125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.46484375" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.53125" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.46484375" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.19921875" style="17"/>
-    <col min="10" max="10" width="13.53125" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="96.53125" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.19921875" style="17"/>
+    <col min="3" max="3" width="13.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="17"/>
+    <col min="10" max="10" width="13.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="96.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:11" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B1" s="18" t="s">
         <v>31</v>
       </c>
@@ -16578,7 +16623,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:11" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="19" t="s">
         <v>27</v>
       </c>
@@ -16604,7 +16649,7 @@
         <v>960.3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="19" t="s">
         <v>28</v>
       </c>
@@ -16630,7 +16675,7 @@
         <v>1663.2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="19" t="s">
         <v>29</v>
       </c>
@@ -16656,7 +16701,7 @@
         <v>777.4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:11" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="J7" s="18" t="s">
         <v>31</v>
       </c>
@@ -16664,7 +16709,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:11" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="J8" s="18" t="s">
         <v>32</v>
       </c>
@@ -16672,7 +16717,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:11" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="J9" s="18" t="s">
         <v>37</v>
       </c>
@@ -16680,7 +16725,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:11" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="J10" s="18" t="s">
         <v>36</v>
       </c>
@@ -16688,7 +16733,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:11" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="J11" s="18" t="s">
         <v>35</v>
       </c>
@@ -16696,7 +16741,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:11" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="J12" s="18" t="s">
         <v>34</v>
       </c>
@@ -16704,7 +16749,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="19.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:11" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="J13" s="18" t="s">
         <v>33</v>
       </c>
@@ -16712,7 +16757,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -16724,20 +16769,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="16.5" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.53125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.53125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.19921875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="19.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.19921875" style="4"/>
+    <col min="1" max="1" width="42.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.1796875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
@@ -16757,7 +16802,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
@@ -16777,7 +16822,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -16797,7 +16842,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>65</v>
       </c>
@@ -16817,7 +16862,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
@@ -16837,7 +16882,7 @@
         <v>1712</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>48</v>
       </c>
@@ -16857,7 +16902,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
@@ -16877,7 +16922,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>68</v>
       </c>
@@ -16897,7 +16942,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>69</v>
       </c>
@@ -16917,7 +16962,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>67</v>
       </c>
@@ -16937,7 +16982,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>66</v>
       </c>
@@ -16969,22 +17014,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C534E5F-56B3-464F-ACD4-646EB824795D}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="16.5" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.53125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.53125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.19921875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="19.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.19921875" style="4"/>
+    <col min="1" max="1" width="34.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="7.90625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.90625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
@@ -17004,12 +17051,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B2" s="5">
-        <v>476.4</v>
+        <v>470.6</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -17024,15 +17071,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B3" s="5">
-        <v>3729</v>
+        <v>3561.8</v>
       </c>
       <c r="C3" s="4">
-        <v>7.83</v>
+        <v>7.57</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
@@ -17044,24 +17091,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B4" s="5">
-        <v>8154.7</v>
+        <v>8413.9</v>
       </c>
       <c r="C4" s="4">
-        <v>17.14</v>
+        <v>17.88</v>
       </c>
       <c r="D4" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
       </c>
       <c r="F4" s="4">
-        <v>33</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="5">
+        <v>7741.4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>16.45</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>